<commit_message>
updated so that tracks with relocation are included
</commit_message>
<xml_diff>
--- a/Bruderer_2001_extracted_from_paper.xlsx
+++ b/Bruderer_2001_extracted_from_paper.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">species</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Turdus merula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accipiter gentilis</t>
   </si>
 </sst>
 </file>
@@ -154,13 +157,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.88"/>
   </cols>
@@ -229,6 +232,17 @@
       </c>
       <c r="C6" s="0" t="n">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>